<commit_message>
Add captcha logic for GA
</commit_message>
<xml_diff>
--- a/APS State Websites v3/Data/Config.xlsx
+++ b/APS State Websites v3/Data/Config.xlsx
@@ -46,7 +46,7 @@
     <x:t>OutputFile</x:t>
   </x:si>
   <x:si>
-    <x:t>Data\Output\output_file_from_03302022.xlsx</x:t>
+    <x:t>Data\Output\output_file_from_07132022.xlsx</x:t>
   </x:si>
   <x:si>
     <x:t>This file is where the automation will write the data to</x:t>
@@ -190,12 +190,747 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="254">
+  <x:cellStyleXfs count="499">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">

</xml_diff>

<commit_message>
Fixed Texas Scraper and Improved Speed.
</commit_message>
<xml_diff>
--- a/APS State Websites v3/Data/Config.xlsx
+++ b/APS State Websites v3/Data/Config.xlsx
@@ -46,7 +46,7 @@
     <x:t>OutputFile</x:t>
   </x:si>
   <x:si>
-    <x:t>Data\Output\output_file_from_08102022.xlsx</x:t>
+    <x:t>Data\Output\output_file_from_08292022.xlsx</x:t>
   </x:si>
   <x:si>
     <x:t>This file is where the automation will write the data to</x:t>
@@ -190,12 +190,369 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="556">
+  <x:cellStyleXfs count="675">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">

</xml_diff>